<commit_message>
feat: count solving times
</commit_message>
<xml_diff>
--- a/raw-data.xlsx
+++ b/raw-data.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rico/Documents/Working/verilock/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rico/Documents/Working/OOPSLA/verilock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6EFE54-2833-6542-9C27-5D6DC1E37146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{328EFD44-B67A-9244-BD4E-B608CFB228B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22980" yWindow="0" windowWidth="15420" windowHeight="21600" xr2:uid="{0E15C672-8EE6-2C4A-9C9F-FD6E491D29AF}"/>
+    <workbookView xWindow="7960" yWindow="500" windowWidth="26380" windowHeight="19780" xr2:uid="{0E15C672-8EE6-2C4A-9C9F-FD6E491D29AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw" sheetId="1" r:id="rId1"/>
     <sheet name="Bar" sheetId="2" r:id="rId2"/>
     <sheet name="Box" sheetId="3" r:id="rId3"/>
+    <sheet name="Channel-Sat" sheetId="5" r:id="rId4"/>
+    <sheet name="Channel-Unsat" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Raw!$A$1:$D$102</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="120">
   <si>
     <t>Case</t>
   </si>
@@ -465,6 +467,3094 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Channel-Sat'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Verilock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Channel-Sat'!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>387</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>498</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Channel-Sat'!$B$2:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>365.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>225.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>183.8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>29.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.400000000000006</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>181.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>398.7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>142</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>33.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>307</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>305.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>366</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>294.7</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>292.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>25.3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>100.4</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>253.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>309.10000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>225.7</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>190.6</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>59.7</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>239</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>135.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>371.3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27.1</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>432.2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>216.5</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>71.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>343.9</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>19.8</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>244.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>297.3</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>232.1</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>258.7</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>363.4</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>35.799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44.8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>293.3</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>158.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>160.6</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>335.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E1DC-4440-B3E7-3F26ECE12730}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Channel-Sat'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Verilock-f</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Channel-Sat'!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>178</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>272</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>293</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>335</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>362</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>379</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>387</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>431</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>435</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>447</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>457</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>464</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>471</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>492</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>498</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Channel-Sat'!$C$2:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>600</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E1DC-4440-B3E7-3F26ECE12730}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1097311264"/>
+        <c:axId val="1097312992"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1097311264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1097312992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1097312992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1097311264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Channel-Unsat'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Verilock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Channel-Unsat'!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1069</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1138</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1234</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1538</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1813</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1827</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1912</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1939</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2059</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2121</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2207</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2258</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2286</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2405</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2498</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2564</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2604</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2687</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2848</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3054</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3104</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3133</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3223</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3231</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3284</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3774</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3864</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4023</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4062</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4087</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4128</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4537</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4613</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4835</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4860</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5097</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5485</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6115</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6642</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Channel-Unsat'!$B$2:$B$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>25.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9.9</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>22.7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29.8</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>19.3</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>23.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>17.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>18.3</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>23.6</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37.4</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>30.3</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>33.6</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>26.7</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>25.3</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>18.3</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>36.299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>25.8</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>40.9</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>23.2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>25.9</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>26.8</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>32.200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>38.799999999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-71C4-7245-9D43-327006752FCA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Channel-Unsat'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Verilock-f</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Channel-Unsat'!$A$2:$A$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>252</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>494</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>687</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1069</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1138</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1234</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1538</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1813</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1827</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1850</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1912</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1939</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2039</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2059</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2121</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2207</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2258</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2286</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2405</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2498</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2564</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2604</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2687</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2848</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3054</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3104</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3133</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3223</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3231</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3284</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3700</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3774</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3864</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4023</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4062</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4087</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4128</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4537</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4613</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4835</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4860</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5097</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5485</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>6115</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>6642</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Channel-Unsat'!$C$2:$C$51</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="50"/>
+                <c:pt idx="0">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39.5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>95.7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>114.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>107.4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28.9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>19.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>17.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>21.6</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>435.3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>59.3</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17.8</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>586.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>35.9</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>502.7</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>57.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-71C4-7245-9D43-327006752FCA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1108846448"/>
+        <c:axId val="1108848176"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1108846448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1108848176"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1108848176"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1108846448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-CN"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{073AD7B4-E2A3-4134-ECCE-486250A1B790}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD3C67F0-1622-2379-D264-A30B8D5DC47F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -767,7 +3857,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2808,7 +5898,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2966,4 +6056,1164 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72276FDC-EF75-2449-9E9F-E1806300024E}">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>365.1</v>
+      </c>
+      <c r="C2">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>225.5</v>
+      </c>
+      <c r="C3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>183.8</v>
+      </c>
+      <c r="C4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>29.8</v>
+      </c>
+      <c r="C5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>69</v>
+      </c>
+      <c r="C6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="C7">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>181.6</v>
+      </c>
+      <c r="C8">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>32</v>
+      </c>
+      <c r="B9">
+        <v>26.1</v>
+      </c>
+      <c r="C9">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>398.7</v>
+      </c>
+      <c r="C10">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11">
+        <v>142</v>
+      </c>
+      <c r="C11">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>65</v>
+      </c>
+      <c r="B12">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="C12">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>71</v>
+      </c>
+      <c r="B13">
+        <v>307</v>
+      </c>
+      <c r="C13">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>73</v>
+      </c>
+      <c r="B14">
+        <v>305.3</v>
+      </c>
+      <c r="C14">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>92</v>
+      </c>
+      <c r="B15">
+        <v>366</v>
+      </c>
+      <c r="C15">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>93</v>
+      </c>
+      <c r="B16">
+        <v>30.1</v>
+      </c>
+      <c r="C16">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>106</v>
+      </c>
+      <c r="B17">
+        <v>294.7</v>
+      </c>
+      <c r="C17">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>108</v>
+      </c>
+      <c r="B18">
+        <v>292.60000000000002</v>
+      </c>
+      <c r="C18">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>113</v>
+      </c>
+      <c r="B19">
+        <v>25.3</v>
+      </c>
+      <c r="C19">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>132</v>
+      </c>
+      <c r="B20">
+        <v>100.4</v>
+      </c>
+      <c r="C20">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>150</v>
+      </c>
+      <c r="B21">
+        <v>253.3</v>
+      </c>
+      <c r="C21">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>154</v>
+      </c>
+      <c r="B22">
+        <v>309.10000000000002</v>
+      </c>
+      <c r="C22">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>158</v>
+      </c>
+      <c r="B23">
+        <v>225.7</v>
+      </c>
+      <c r="C23">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>178</v>
+      </c>
+      <c r="B24">
+        <v>190.6</v>
+      </c>
+      <c r="C24">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>218</v>
+      </c>
+      <c r="B25">
+        <v>59.7</v>
+      </c>
+      <c r="C25">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>219</v>
+      </c>
+      <c r="B26">
+        <v>239</v>
+      </c>
+      <c r="C26">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>272</v>
+      </c>
+      <c r="B27">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="C27">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>272</v>
+      </c>
+      <c r="B28">
+        <v>135.6</v>
+      </c>
+      <c r="C28">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>292</v>
+      </c>
+      <c r="B29">
+        <v>371.3</v>
+      </c>
+      <c r="C29">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>293</v>
+      </c>
+      <c r="B30">
+        <v>27.1</v>
+      </c>
+      <c r="C30">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>330</v>
+      </c>
+      <c r="B31">
+        <v>432.2</v>
+      </c>
+      <c r="C31">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>334</v>
+      </c>
+      <c r="B32">
+        <v>216.5</v>
+      </c>
+      <c r="C32">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>335</v>
+      </c>
+      <c r="B33">
+        <v>71.5</v>
+      </c>
+      <c r="C33">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>340</v>
+      </c>
+      <c r="B34">
+        <v>343.9</v>
+      </c>
+      <c r="C34">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>344</v>
+      </c>
+      <c r="B35">
+        <v>19.8</v>
+      </c>
+      <c r="C35">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>362</v>
+      </c>
+      <c r="B36">
+        <v>17.8</v>
+      </c>
+      <c r="C36">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>379</v>
+      </c>
+      <c r="B37">
+        <v>244.5</v>
+      </c>
+      <c r="C37">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>387</v>
+      </c>
+      <c r="B38">
+        <v>297.3</v>
+      </c>
+      <c r="C38">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>431</v>
+      </c>
+      <c r="B39">
+        <v>232.1</v>
+      </c>
+      <c r="C39">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>435</v>
+      </c>
+      <c r="B40">
+        <v>60</v>
+      </c>
+      <c r="C40">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>447</v>
+      </c>
+      <c r="B41">
+        <v>29.5</v>
+      </c>
+      <c r="C41">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>450</v>
+      </c>
+      <c r="B42">
+        <v>258.7</v>
+      </c>
+      <c r="C42">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>450</v>
+      </c>
+      <c r="B43">
+        <v>363.4</v>
+      </c>
+      <c r="C43">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>455</v>
+      </c>
+      <c r="B44">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="C44">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>457</v>
+      </c>
+      <c r="B45">
+        <v>44.8</v>
+      </c>
+      <c r="C45">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>464</v>
+      </c>
+      <c r="B46">
+        <v>293.3</v>
+      </c>
+      <c r="C46">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>471</v>
+      </c>
+      <c r="B47">
+        <v>158.30000000000001</v>
+      </c>
+      <c r="C47">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>471</v>
+      </c>
+      <c r="B48">
+        <v>22.5</v>
+      </c>
+      <c r="C48">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>483</v>
+      </c>
+      <c r="B49">
+        <v>160.6</v>
+      </c>
+      <c r="C49">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>492</v>
+      </c>
+      <c r="B50">
+        <v>300</v>
+      </c>
+      <c r="C50">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>498</v>
+      </c>
+      <c r="B51">
+        <v>335.8</v>
+      </c>
+      <c r="C51">
+        <v>600</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C51">
+    <sortCondition ref="A2:A51"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1630982E-F949-6B47-AEB2-83655781C9ED}">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="P34" sqref="P34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>252</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="C2">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>344</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>455</v>
+      </c>
+      <c r="B4">
+        <v>2.9</v>
+      </c>
+      <c r="C4">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>494</v>
+      </c>
+      <c r="B5">
+        <v>2.6</v>
+      </c>
+      <c r="C5">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>687</v>
+      </c>
+      <c r="B6">
+        <v>4.3</v>
+      </c>
+      <c r="C6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>739</v>
+      </c>
+      <c r="B7">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="C7">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>810</v>
+      </c>
+      <c r="B8">
+        <v>5.2</v>
+      </c>
+      <c r="C8">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>847</v>
+      </c>
+      <c r="B9">
+        <v>5.6</v>
+      </c>
+      <c r="C9">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1069</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1138</v>
+      </c>
+      <c r="B11">
+        <v>9.4</v>
+      </c>
+      <c r="C11">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1234</v>
+      </c>
+      <c r="B12">
+        <v>25.3</v>
+      </c>
+      <c r="C12">
+        <v>95.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1538</v>
+      </c>
+      <c r="B13">
+        <v>23.8</v>
+      </c>
+      <c r="C13">
+        <v>16.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1813</v>
+      </c>
+      <c r="B14">
+        <v>12.7</v>
+      </c>
+      <c r="C14">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1827</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>114.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1850</v>
+      </c>
+      <c r="B16">
+        <v>9.9</v>
+      </c>
+      <c r="C16">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1912</v>
+      </c>
+      <c r="B17">
+        <v>11.8</v>
+      </c>
+      <c r="C17">
+        <v>107.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1939</v>
+      </c>
+      <c r="B18">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2039</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2059</v>
+      </c>
+      <c r="B20">
+        <v>22.7</v>
+      </c>
+      <c r="C20">
+        <v>28.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2121</v>
+      </c>
+      <c r="B21">
+        <v>10.4</v>
+      </c>
+      <c r="C21">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2207</v>
+      </c>
+      <c r="B22">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2258</v>
+      </c>
+      <c r="B23">
+        <v>12.6</v>
+      </c>
+      <c r="C23">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2286</v>
+      </c>
+      <c r="B24">
+        <v>11.9</v>
+      </c>
+      <c r="C24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2405</v>
+      </c>
+      <c r="B25">
+        <v>13.4</v>
+      </c>
+      <c r="C25">
+        <v>20.399999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2498</v>
+      </c>
+      <c r="B26">
+        <v>12.8</v>
+      </c>
+      <c r="C26">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2564</v>
+      </c>
+      <c r="B27">
+        <v>29.8</v>
+      </c>
+      <c r="C27">
+        <v>21.6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2604</v>
+      </c>
+      <c r="B28">
+        <v>14.9</v>
+      </c>
+      <c r="C28">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2687</v>
+      </c>
+      <c r="B29">
+        <v>14.7</v>
+      </c>
+      <c r="C29">
+        <v>435.3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2848</v>
+      </c>
+      <c r="B30">
+        <v>15</v>
+      </c>
+      <c r="C30">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>3054</v>
+      </c>
+      <c r="B31">
+        <v>16.8</v>
+      </c>
+      <c r="C31">
+        <v>59.3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3104</v>
+      </c>
+      <c r="B32">
+        <v>14.4</v>
+      </c>
+      <c r="C32">
+        <v>17.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3133</v>
+      </c>
+      <c r="B33">
+        <v>19.3</v>
+      </c>
+      <c r="C33">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3223</v>
+      </c>
+      <c r="B34">
+        <v>23.7</v>
+      </c>
+      <c r="C34">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3231</v>
+      </c>
+      <c r="B35">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="C35">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3284</v>
+      </c>
+      <c r="B36">
+        <v>18.3</v>
+      </c>
+      <c r="C36">
+        <v>586.20000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3700</v>
+      </c>
+      <c r="B37">
+        <v>23.6</v>
+      </c>
+      <c r="C37">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3774</v>
+      </c>
+      <c r="B38">
+        <v>37.4</v>
+      </c>
+      <c r="C38">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3864</v>
+      </c>
+      <c r="B39">
+        <v>30.3</v>
+      </c>
+      <c r="C39">
+        <v>35.9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4023</v>
+      </c>
+      <c r="B40">
+        <v>33.6</v>
+      </c>
+      <c r="C40">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>4062</v>
+      </c>
+      <c r="B41">
+        <v>26.7</v>
+      </c>
+      <c r="C41">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>4087</v>
+      </c>
+      <c r="B42">
+        <v>25.3</v>
+      </c>
+      <c r="C42">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>4128</v>
+      </c>
+      <c r="B43">
+        <v>18.3</v>
+      </c>
+      <c r="C43">
+        <v>502.7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>4537</v>
+      </c>
+      <c r="B44">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="C44">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>4613</v>
+      </c>
+      <c r="B45">
+        <v>25.8</v>
+      </c>
+      <c r="C45">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>4835</v>
+      </c>
+      <c r="B46">
+        <v>40.9</v>
+      </c>
+      <c r="C46">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>4860</v>
+      </c>
+      <c r="B47">
+        <v>23.2</v>
+      </c>
+      <c r="C47">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>5097</v>
+      </c>
+      <c r="B48">
+        <v>25.9</v>
+      </c>
+      <c r="C48">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>5485</v>
+      </c>
+      <c r="B49">
+        <v>26.8</v>
+      </c>
+      <c r="C49">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>6115</v>
+      </c>
+      <c r="B50">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="C50">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>6642</v>
+      </c>
+      <c r="B51">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="C51">
+        <v>57.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C51">
+    <sortCondition ref="A2:A51"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>